<commit_message>
Agrego comienzo del informe (subnetting, diagrama de la red y configuracion de los routers)
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/documentacion/Configuracion Ruters.xlsx
+++ b/ tp-distribuidos-grupo3/documentacion/Configuracion Ruters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="750" yWindow="615" windowWidth="16215" windowHeight="7620"/>
@@ -432,20 +432,20 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,14 +482,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD5A6BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -672,12 +666,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -688,34 +689,26 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -727,22 +720,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -754,8 +735,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,7 +1078,7 @@
   <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1073,1998 +1090,2003 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="13"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="14" t="s">
         <v>132</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="14" t="s">
         <v>63</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="18"/>
+      <c r="E31" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H31" s="12"/>
-      <c r="I31" s="11" t="s">
+      <c r="H31" s="18"/>
+      <c r="I31" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="17" t="s">
         <v>88</v>
       </c>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15" t="s">
+      <c r="D32" s="18"/>
+      <c r="E32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="15" t="s">
+      <c r="H32" s="18"/>
+      <c r="I32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="19" t="s">
         <v>91</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="2" t="s">
+      <c r="D33" s="18"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="2" t="s">
+      <c r="H33" s="18"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="2" t="s">
+      <c r="D34" s="18"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="2" t="s">
+      <c r="H34" s="18"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="19" t="s">
         <v>91</v>
       </c>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="2" t="s">
+      <c r="D35" s="18"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="2" t="s">
+      <c r="H35" s="18"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="19" t="s">
         <v>91</v>
       </c>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="2" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="2" t="s">
+      <c r="D36" s="18"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H36" s="12"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="2" t="s">
+      <c r="H36" s="18"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="19" t="s">
         <v>102</v>
       </c>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="8"/>
+      <c r="B37" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="2" t="s">
+      <c r="D37" s="18"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="12"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="2" t="s">
+      <c r="H37" s="18"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K37" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="2" t="s">
+      <c r="D38" s="18"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="2" t="s">
+      <c r="H38" s="18"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="8"/>
+      <c r="B39" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="2" t="s">
+      <c r="D39" s="18"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="2" t="s">
+      <c r="H39" s="18"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="2" t="s">
+      <c r="D40" s="18"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H40" s="12"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="2" t="s">
+      <c r="H40" s="18"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" s="19" t="s">
         <v>91</v>
       </c>
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="2" t="s">
+      <c r="D41" s="18"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="12"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="2" t="s">
+      <c r="H41" s="18"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="K41" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="8"/>
+      <c r="B42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="2" t="s">
+      <c r="D42" s="18"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H42" s="12"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="2" t="s">
+      <c r="H42" s="18"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="K42" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="8"/>
+      <c r="B43" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="2" t="s">
+      <c r="D43" s="18"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H43" s="12"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="2" t="s">
+      <c r="H43" s="18"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="K43" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="16"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="2" t="s">
+      <c r="D44" s="18"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="2" t="s">
+      <c r="H44" s="18"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="K44" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
-      <c r="B45" s="2" t="s">
+      <c r="A45" s="8"/>
+      <c r="B45" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="2" t="s">
+      <c r="D45" s="18"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="2" t="s">
+      <c r="H45" s="18"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="K45" s="19" t="s">
         <v>115</v>
       </c>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
-      <c r="B46" s="2" t="s">
+      <c r="A46" s="8"/>
+      <c r="B46" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="2" t="s">
+      <c r="D46" s="18"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="2" t="s">
+      <c r="H46" s="18"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="K46" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="8"/>
+      <c r="B47" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="2" t="s">
+      <c r="D47" s="18"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="2" t="s">
+      <c r="H47" s="18"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K47" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="B48" s="2" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="2" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H48" s="12"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="2" t="s">
+      <c r="H48" s="18"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="2" t="s">
+      <c r="A49" s="20"/>
+      <c r="B49" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="2" t="s">
+      <c r="D49" s="18"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="H49" s="12"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="2" t="s">
+      <c r="H49" s="18"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="K49" s="19" t="s">
         <v>102</v>
       </c>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11" t="s">
+      <c r="D51" s="18"/>
+      <c r="E51" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="11" t="s">
+      <c r="H51" s="18"/>
+      <c r="I51" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J51" s="11" t="s">
+      <c r="J51" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K51" s="11" t="s">
+      <c r="K51" s="17" t="s">
         <v>88</v>
       </c>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="15" t="s">
+      <c r="D52" s="18"/>
+      <c r="E52" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="15" t="s">
+      <c r="H52" s="18"/>
+      <c r="I52" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="J52" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="K52" s="19" t="s">
         <v>121</v>
       </c>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="16"/>
-      <c r="B53" s="2" t="s">
+      <c r="A53" s="8"/>
+      <c r="B53" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="2" t="s">
+      <c r="D53" s="18"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="2" t="s">
+      <c r="H53" s="18"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="K53" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="2" t="s">
+      <c r="A54" s="8"/>
+      <c r="B54" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="2" t="s">
+      <c r="D54" s="18"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H54" s="12"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="2" t="s">
+      <c r="H54" s="18"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="K54" s="19" t="s">
         <v>121</v>
       </c>
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16"/>
-      <c r="B55" s="2" t="s">
+      <c r="A55" s="8"/>
+      <c r="B55" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="2" t="s">
+      <c r="D55" s="18"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="2" t="s">
+      <c r="H55" s="18"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="K55" s="19" t="s">
         <v>121</v>
       </c>
       <c r="L55" s="1"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="16"/>
-      <c r="B56" s="2" t="s">
+      <c r="A56" s="8"/>
+      <c r="B56" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="2" t="s">
+      <c r="D56" s="18"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="2" t="s">
+      <c r="H56" s="18"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="K56" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="16"/>
-      <c r="B57" s="2" t="s">
+      <c r="A57" s="8"/>
+      <c r="B57" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="2" t="s">
+      <c r="D57" s="18"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="2" t="s">
+      <c r="H57" s="18"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="K57" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="16"/>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="8"/>
+      <c r="B58" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="2" t="s">
+      <c r="D58" s="18"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H58" s="12"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="2" t="s">
+      <c r="H58" s="18"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="K58" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="16"/>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="8"/>
+      <c r="B59" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="2" t="s">
+      <c r="D59" s="18"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H59" s="12"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="2" t="s">
+      <c r="H59" s="18"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="K59" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="16"/>
-      <c r="B60" s="2" t="s">
+      <c r="A60" s="8"/>
+      <c r="B60" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="2" t="s">
+      <c r="D60" s="18"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H60" s="12"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="2" t="s">
+      <c r="H60" s="18"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="K60" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L60" s="1"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="16"/>
-      <c r="B61" s="2" t="s">
+      <c r="A61" s="8"/>
+      <c r="B61" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="2" t="s">
+      <c r="D61" s="18"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H61" s="12"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="2" t="s">
+      <c r="H61" s="18"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="K61" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="16"/>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="8"/>
+      <c r="B62" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="2" t="s">
+      <c r="D62" s="18"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H62" s="12"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="2" t="s">
+      <c r="H62" s="18"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="K62" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L62" s="1"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="16"/>
-      <c r="B63" s="2" t="s">
+      <c r="A63" s="8"/>
+      <c r="B63" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="2" t="s">
+      <c r="D63" s="18"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H63" s="12"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="2" t="s">
+      <c r="H63" s="18"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="K63" s="2" t="s">
+      <c r="K63" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L63" s="1"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="16"/>
-      <c r="B64" s="2" t="s">
+      <c r="A64" s="8"/>
+      <c r="B64" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="2" t="s">
+      <c r="D64" s="18"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H64" s="12"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="2" t="s">
+      <c r="H64" s="18"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="K64" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L64" s="1"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="16"/>
-      <c r="B65" s="2" t="s">
+      <c r="A65" s="8"/>
+      <c r="B65" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="2" t="s">
+      <c r="D65" s="18"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H65" s="12"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="2" t="s">
+      <c r="H65" s="18"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="K65" s="19" t="s">
         <v>115</v>
       </c>
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="16"/>
-      <c r="B66" s="2" t="s">
+      <c r="A66" s="8"/>
+      <c r="B66" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="2" t="s">
+      <c r="D66" s="18"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H66" s="12"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="2" t="s">
+      <c r="H66" s="18"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="K66" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="16"/>
-      <c r="B67" s="2" t="s">
+      <c r="A67" s="8"/>
+      <c r="B67" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D67" s="12"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="2" t="s">
+      <c r="D67" s="18"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H67" s="12"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="2" t="s">
+      <c r="H67" s="18"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="K67" s="2" t="s">
+      <c r="K67" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="2" t="s">
+      <c r="A68" s="9"/>
+      <c r="B68" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="2" t="s">
+      <c r="D68" s="18"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H68" s="12"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="2" t="s">
+      <c r="H68" s="18"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="K68" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="2" t="s">
+      <c r="A69" s="20"/>
+      <c r="B69" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="12"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="2" t="s">
+      <c r="D69" s="18"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H69" s="12"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="2" t="s">
+      <c r="H69" s="18"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="K69" s="19" t="s">
         <v>124</v>
       </c>
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D71" s="12"/>
-      <c r="E71" s="11" t="s">
+      <c r="D71" s="18"/>
+      <c r="E71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G71" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H71" s="12"/>
-      <c r="I71" s="11" t="s">
+      <c r="H71" s="18"/>
+      <c r="I71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J71" s="11" t="s">
+      <c r="J71" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K71" s="11" t="s">
+      <c r="K71" s="17" t="s">
         <v>88</v>
       </c>
       <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="15" t="s">
+      <c r="D72" s="18"/>
+      <c r="E72" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H72" s="12"/>
-      <c r="I72" s="15" t="s">
+      <c r="H72" s="18"/>
+      <c r="I72" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J72" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K72" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="16"/>
-      <c r="B73" s="2" t="s">
+      <c r="A73" s="8"/>
+      <c r="B73" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D73" s="12"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="2" t="s">
+      <c r="D73" s="18"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H73" s="12"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="2" t="s">
+      <c r="H73" s="18"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="K73" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L73" s="1"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="16"/>
-      <c r="B74" s="2" t="s">
+      <c r="A74" s="8"/>
+      <c r="B74" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D74" s="12"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="2" t="s">
+      <c r="D74" s="18"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H74" s="12"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="2" t="s">
+      <c r="H74" s="18"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="K74" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="16"/>
-      <c r="B75" s="2" t="s">
+      <c r="A75" s="8"/>
+      <c r="B75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="12"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="2" t="s">
+      <c r="D75" s="18"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H75" s="12"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="2" t="s">
+      <c r="H75" s="18"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="K75" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L75" s="1"/>
     </row>
     <row r="76" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="16"/>
-      <c r="B76" s="2" t="s">
+      <c r="A76" s="8"/>
+      <c r="B76" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D76" s="12"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="2" t="s">
+      <c r="D76" s="18"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H76" s="12"/>
-      <c r="I76" s="16"/>
-      <c r="J76" s="2" t="s">
+      <c r="H76" s="18"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="K76" s="19" t="s">
         <v>102</v>
       </c>
       <c r="L76" s="1"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A77" s="16"/>
-      <c r="B77" s="2" t="s">
+      <c r="A77" s="8"/>
+      <c r="B77" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D77" s="12"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="2" t="s">
+      <c r="D77" s="18"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H77" s="12"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="2" t="s">
+      <c r="H77" s="18"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="K77" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L77" s="1"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A78" s="16"/>
-      <c r="B78" s="2" t="s">
+      <c r="A78" s="8"/>
+      <c r="B78" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="2" t="s">
+      <c r="D78" s="18"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H78" s="12"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="2" t="s">
+      <c r="H78" s="18"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K78" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="16"/>
-      <c r="B79" s="2" t="s">
+      <c r="A79" s="8"/>
+      <c r="B79" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D79" s="12"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="2" t="s">
+      <c r="D79" s="18"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H79" s="12"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="2" t="s">
+      <c r="H79" s="18"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="K79" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L79" s="1"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" s="16"/>
-      <c r="B80" s="2" t="s">
+      <c r="A80" s="8"/>
+      <c r="B80" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="2" t="s">
+      <c r="D80" s="18"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G80" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H80" s="12"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="2" t="s">
+      <c r="H80" s="18"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K80" s="19" t="s">
         <v>123</v>
       </c>
       <c r="L80" s="1"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" s="16"/>
-      <c r="B81" s="2" t="s">
+      <c r="A81" s="8"/>
+      <c r="B81" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D81" s="12"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="2" t="s">
+      <c r="D81" s="18"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H81" s="12"/>
-      <c r="I81" s="16"/>
-      <c r="J81" s="2" t="s">
+      <c r="H81" s="18"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="K81" s="2" t="s">
+      <c r="K81" s="19" t="s">
         <v>94</v>
       </c>
       <c r="L81" s="1"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" s="16"/>
-      <c r="B82" s="2" t="s">
+      <c r="A82" s="8"/>
+      <c r="B82" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="2" t="s">
+      <c r="D82" s="18"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H82" s="12"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="2" t="s">
+      <c r="H82" s="18"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="K82" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A83" s="16"/>
-      <c r="B83" s="2" t="s">
+      <c r="A83" s="8"/>
+      <c r="B83" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D83" s="12"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="2" t="s">
+      <c r="D83" s="18"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H83" s="12"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="2" t="s">
+      <c r="H83" s="18"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="K83" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L83" s="1"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A84" s="16"/>
-      <c r="B84" s="2" t="s">
+      <c r="A84" s="8"/>
+      <c r="B84" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="12"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="2" t="s">
+      <c r="D84" s="18"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H84" s="12"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="2" t="s">
+      <c r="H84" s="18"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="K84" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L84" s="1"/>
     </row>
     <row r="85" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A85" s="16"/>
-      <c r="B85" s="2" t="s">
+      <c r="A85" s="8"/>
+      <c r="B85" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D85" s="12"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="2" t="s">
+      <c r="D85" s="18"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H85" s="12"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="2" t="s">
+      <c r="H85" s="18"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="K85" s="2" t="s">
+      <c r="K85" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L85" s="1"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="16"/>
-      <c r="B86" s="2" t="s">
+      <c r="A86" s="8"/>
+      <c r="B86" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D86" s="12"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="2" t="s">
+      <c r="D86" s="18"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H86" s="12"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="2" t="s">
+      <c r="H86" s="18"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="K86" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L86" s="1"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A87" s="16"/>
-      <c r="B87" s="2" t="s">
+      <c r="A87" s="8"/>
+      <c r="B87" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D87" s="12"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="2" t="s">
+      <c r="D87" s="18"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H87" s="12"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="2" t="s">
+      <c r="H87" s="18"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="K87" s="2" t="s">
+      <c r="K87" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L87" s="1"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="2" t="s">
+      <c r="A88" s="9"/>
+      <c r="B88" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D88" s="12"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="2" t="s">
+      <c r="D88" s="18"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H88" s="12"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="2" t="s">
+      <c r="H88" s="18"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="K88" s="19" t="s">
         <v>105</v>
       </c>
       <c r="L88" s="1"/>
     </row>
     <row r="89" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="2" t="s">
+      <c r="A89" s="20"/>
+      <c r="B89" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D89" s="12"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="2" t="s">
+      <c r="D89" s="18"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G89" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H89" s="12"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="2" t="s">
+      <c r="H89" s="18"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K89" s="19" t="s">
         <v>124</v>
       </c>
       <c r="L89" s="1"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="A72:A89"/>
     <mergeCell ref="E72:E89"/>
     <mergeCell ref="I72:I89"/>
@@ -3076,5 +3098,6 @@
     <mergeCell ref="I52:I69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>